<commit_message>
feat: enhance file upload validation and improve user feedback
</commit_message>
<xml_diff>
--- a/public/templates/template-excel.xlsx
+++ b/public/templates/template-excel.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{248A1183-981E-463F-83C5-5BC0E5A4DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -96,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -117,6 +121,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -288,39 +293,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,90 +657,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="2"/>
-    <col min="3" max="3" width="20.7109375" style="6"/>
-    <col min="4" max="4" width="20.7109375" style="3"/>
-    <col min="5" max="8" width="20.7109375" style="2"/>
-    <col min="9" max="9" width="20.7109375" style="4"/>
-    <col min="10" max="11" width="20.7109375" style="2"/>
-    <col min="12" max="13" width="20.7109375" style="6"/>
-    <col min="14" max="15" width="20.7109375" style="2"/>
-    <col min="16" max="16" width="20.7109375" style="4"/>
-    <col min="17" max="20" width="20.7109375" style="2"/>
-    <col min="21" max="21" width="20.7109375" style="4"/>
+    <col min="1" max="2" width="20.69921875" style="2"/>
+    <col min="3" max="3" width="20.69921875" style="6"/>
+    <col min="4" max="4" width="20.69921875" style="3"/>
+    <col min="5" max="8" width="20.69921875" style="2"/>
+    <col min="9" max="9" width="20.69921875" style="4"/>
+    <col min="10" max="11" width="20.69921875" style="2"/>
+    <col min="12" max="13" width="20.69921875" style="6"/>
+    <col min="14" max="15" width="20.69921875" style="2"/>
+    <col min="16" max="16" width="20.69921875" style="4"/>
+    <col min="17" max="20" width="20.69921875" style="2"/>
+    <col min="21" max="21" width="20.69921875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="30.75">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:27" ht="28.8">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="19" t="s">
         <v>19</v>
       </c>
       <c r="V1" s="13"/>
@@ -753,7 +756,7 @@
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
       <c r="X2" s="14"/>
-      <c r="Y2" s="15"/>
+      <c r="Y2" s="23"/>
       <c r="Z2" s="14"/>
       <c r="AA2" s="14"/>
     </row>
@@ -765,7 +768,7 @@
       <c r="V3" s="14"/>
       <c r="W3" s="14"/>
       <c r="X3" s="14"/>
-      <c r="Y3" s="15"/>
+      <c r="Y3" s="23"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="14"/>
     </row>
@@ -777,7 +780,7 @@
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
       <c r="X4" s="14"/>
-      <c r="Y4" s="15"/>
+      <c r="Y4" s="23"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="14"/>
     </row>
@@ -789,7 +792,7 @@
       <c r="V5" s="14"/>
       <c r="W5" s="14"/>
       <c r="X5" s="14"/>
-      <c r="Y5" s="15"/>
+      <c r="Y5" s="23"/>
       <c r="Z5" s="14"/>
       <c r="AA5" s="14"/>
     </row>
@@ -800,7 +803,7 @@
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
-      <c r="Y6" s="15"/>
+      <c r="Y6" s="23"/>
       <c r="Z6" s="14"/>
       <c r="AA6" s="14"/>
     </row>
@@ -811,7 +814,7 @@
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
       <c r="X7" s="14"/>
-      <c r="Y7" s="15"/>
+      <c r="Y7" s="23"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="14"/>
     </row>
@@ -822,7 +825,7 @@
       <c r="V8" s="14"/>
       <c r="W8" s="14"/>
       <c r="X8" s="14"/>
-      <c r="Y8" s="15"/>
+      <c r="Y8" s="23"/>
       <c r="Z8" s="14"/>
       <c r="AA8" s="14"/>
     </row>
@@ -834,7 +837,7 @@
       <c r="V9" s="14"/>
       <c r="W9" s="14"/>
       <c r="X9" s="14"/>
-      <c r="Y9" s="15"/>
+      <c r="Y9" s="23"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="14"/>
     </row>
@@ -845,7 +848,7 @@
       <c r="V10" s="14"/>
       <c r="W10" s="14"/>
       <c r="X10" s="14"/>
-      <c r="Y10" s="16"/>
+      <c r="Y10" s="24"/>
       <c r="Z10" s="14"/>
       <c r="AA10" s="14"/>
     </row>
@@ -856,7 +859,7 @@
       <c r="V11" s="14"/>
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
-      <c r="Y11" s="16"/>
+      <c r="Y11" s="24"/>
       <c r="Z11" s="14"/>
       <c r="AA11" s="14"/>
     </row>
@@ -864,7 +867,7 @@
       <c r="V12" s="14"/>
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
-      <c r="Y12" s="16"/>
+      <c r="Y12" s="24"/>
       <c r="Z12" s="14"/>
       <c r="AA12" s="14"/>
     </row>
@@ -872,7 +875,7 @@
       <c r="V13" s="14"/>
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
-      <c r="Y13" s="15"/>
+      <c r="Y13" s="23"/>
       <c r="Z13" s="14"/>
       <c r="AA13" s="14"/>
     </row>
@@ -881,7 +884,7 @@
       <c r="V14" s="14"/>
       <c r="W14" s="14"/>
       <c r="X14" s="14"/>
-      <c r="Y14" s="15"/>
+      <c r="Y14" s="23"/>
       <c r="Z14" s="14"/>
       <c r="AA14" s="14"/>
     </row>
@@ -894,7 +897,7 @@
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
       <c r="X15" s="14"/>
-      <c r="Y15" s="15"/>
+      <c r="Y15" s="23"/>
       <c r="Z15" s="14"/>
       <c r="AA15" s="14"/>
     </row>
@@ -907,7 +910,7 @@
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
       <c r="X16" s="14"/>
-      <c r="Y16" s="15"/>
+      <c r="Y16" s="23"/>
       <c r="Z16" s="14"/>
       <c r="AA16" s="14"/>
     </row>
@@ -916,7 +919,7 @@
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
-      <c r="Y17" s="15"/>
+      <c r="Y17" s="23"/>
       <c r="Z17" s="14"/>
       <c r="AA17" s="14"/>
     </row>
@@ -929,7 +932,7 @@
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
       <c r="X18" s="14"/>
-      <c r="Y18" s="15"/>
+      <c r="Y18" s="23"/>
       <c r="Z18" s="14"/>
       <c r="AA18" s="14"/>
     </row>
@@ -938,7 +941,7 @@
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
       <c r="X19" s="14"/>
-      <c r="Y19" s="15"/>
+      <c r="Y19" s="23"/>
       <c r="Z19" s="14"/>
       <c r="AA19" s="14"/>
     </row>
@@ -1018,33 +1021,33 @@
     <mergeCell ref="Y10:Y12"/>
   </mergeCells>
   <dataValidations count="11">
-    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="El carnet de identidad debe tener mas de 7 digitos" sqref="V1 S1 L1 C1" xr:uid="{BBEE65DE-0ADC-43B0-8B9B-62DB40C3F98F}">
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="El carnet de identidad debe tener mas de 7 digitos" sqref="V1 S1 L1 C1">
       <formula1>7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O14:O33 P49:P1048576 P43:P45 P34:P37 O45 O1:O11" xr:uid="{6A11C7CC-96F5-4E1A-BDEE-CD15EEA35701}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O14:O33 P49:P1048576 P43:P45 P34:P37 O45 O1:O11">
       <formula1>$AA$2:$AA$7</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="El estudiante debe haber nacido despues de 2020" sqref="D14:D37 D43:D45 D49:D1048576 D1:D11" xr:uid="{CB5701E9-676D-4641-8B84-FB6043B97A1F}">
+    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="El estudiante debe haber nacido despues de 2020" sqref="D14:D37 D43:D45 D49:D1048576 D1:D11">
       <formula1>43831</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="CI duplicado" error="No se permiten CI duplicados" promptTitle="Correo Electronico" sqref="E14:E37 E43:E45 E49:E1048576 E1:E11" xr:uid="{4A0E37A0-6E8F-44E5-BDED-F6381E79E1E6}"/>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M14:M37 M43:M45 M49:M1048576 M2:M11" xr:uid="{AD86BCCD-92E7-47F0-ABB2-699E86472C61}">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="CI duplicado" error="No se permiten CI duplicados" promptTitle="Correo Electronico" sqref="E14:E37 E43:E45 E49:E1048576 E1:E11"/>
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M14:M37 M43:M45 M49:M1048576 M2:M11">
       <formula1>8</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F37 F43:F45 F49:F1048576 F1:F11" xr:uid="{2B01859B-37EE-43F4-A414-49875F3A4FFA}">
+    <dataValidation type="list" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F37 F43:F45 F49:F1048576 F1:F11">
       <formula1>"Chuquisaca ,La Paz ,Cochabamba ,Oruro ,Potosí ,Tarija ,Santa Cruz ,Beni ,Pando"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O34:O37 O43:O45 O49:O1048576 O2:O11" xr:uid="{30819BE1-2A1E-41FB-AEB1-25FE82C40BFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O34:O37 O43:O45 O49:O1048576 O2:O11">
       <formula1>"Madre, Padre, Tutor"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P11" xr:uid="{86A61FC6-F016-4105-A21B-6A55C84A8CE0}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{FE86766E-BDB7-4A94-BB60-586AE74B3613}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P11"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
       <formula1>"3ro de Primaria, 4to de Primaria, 5to de Primaria, 1ro de Secundaria, 2do de Secundaria, 3ro de Secundaria, 4to de Secundaria, 5to de Secundaria, 6to de Secundaria"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="El carnet de identidad debe tener mas de 7 digitos" sqref="L2:L1048576" xr:uid="{74836F22-1F21-47A9-8F0A-093109D4621E}">
+    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="El carnet de identidad debe tener mas de 7 digitos" sqref="L2:L1048576">
       <formula1>7</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 S2:S1048576" xr:uid="{841C7882-EB65-4DBF-80F1-9A8A208883D9}">
+    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 S2:S1048576">
       <formula1>7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>